<commit_message>
Reprocess rhyolitic glasses and update summary figure
</commit_message>
<xml_diff>
--- a/data/processed/rhyolitic_glasses/calczaf_files/calczaf_oxides_summary.xlsx
+++ b/data/processed/rhyolitic_glasses/calczaf_files/calczaf_oxides_summary.xlsx
@@ -566,10 +566,10 @@
         <v>5.45</v>
       </c>
       <c r="K2">
-        <v>11.904</v>
+        <v>11.864</v>
       </c>
       <c r="L2">
-        <v>0.516</v>
+        <v>0.556</v>
       </c>
       <c r="M2">
         <v>0.05</v>
@@ -610,10 +610,10 @@
         <v>5.45</v>
       </c>
       <c r="K3">
-        <v>11.539</v>
+        <v>11.471</v>
       </c>
       <c r="L3">
-        <v>0.881</v>
+        <v>0.948</v>
       </c>
       <c r="M3">
         <v>0.05</v>
@@ -654,10 +654,10 @@
         <v>5.45</v>
       </c>
       <c r="K4">
-        <v>11.358</v>
+        <v>11.277</v>
       </c>
       <c r="L4">
-        <v>1.061</v>
+        <v>1.143</v>
       </c>
       <c r="M4">
         <v>0.05</v>
@@ -698,10 +698,10 @@
         <v>5.4</v>
       </c>
       <c r="K5">
-        <v>13.226</v>
+        <v>13.211</v>
       </c>
       <c r="L5">
-        <v>0.203</v>
+        <v>0.219</v>
       </c>
       <c r="M5">
         <v>0.03</v>
@@ -742,10 +742,10 @@
         <v>5.4</v>
       </c>
       <c r="K6">
-        <v>12.873</v>
+        <v>12.828</v>
       </c>
       <c r="L6">
-        <v>0.556</v>
+        <v>0.602</v>
       </c>
       <c r="M6">
         <v>0.03</v>
@@ -786,10 +786,10 @@
         <v>5.4</v>
       </c>
       <c r="K7">
-        <v>12.76</v>
+        <v>12.705</v>
       </c>
       <c r="L7">
-        <v>0.67</v>
+        <v>0.725</v>
       </c>
       <c r="M7">
         <v>0.03</v>
@@ -830,10 +830,10 @@
         <v>6</v>
       </c>
       <c r="K8">
-        <v>7.866</v>
+        <v>7.82</v>
       </c>
       <c r="L8">
-        <v>0.603</v>
+        <v>0.649</v>
       </c>
       <c r="M8">
         <v>0.06</v>
@@ -874,10 +874,10 @@
         <v>6</v>
       </c>
       <c r="K9">
-        <v>7.495</v>
+        <v>7.417</v>
       </c>
       <c r="L9">
-        <v>0.975</v>
+        <v>1.052</v>
       </c>
       <c r="M9">
         <v>0.06</v>
@@ -918,10 +918,10 @@
         <v>6</v>
       </c>
       <c r="K10">
-        <v>7.295</v>
+        <v>7.202</v>
       </c>
       <c r="L10">
-        <v>1.174</v>
+        <v>1.267</v>
       </c>
       <c r="M10">
         <v>0.06</v>
@@ -1016,10 +1016,10 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0.031</v>
+        <v>0.034</v>
       </c>
       <c r="L2">
-        <v>0.031</v>
+        <v>0.034</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1060,10 +1060,10 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0.035</v>
+        <v>0.037</v>
       </c>
       <c r="L3">
-        <v>0.035</v>
+        <v>0.037</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1104,10 +1104,10 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0.043</v>
+        <v>0.044</v>
       </c>
       <c r="L4">
-        <v>0.043</v>
+        <v>0.044</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -1148,10 +1148,10 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0.1</v>
+        <v>0.108</v>
       </c>
       <c r="L5">
-        <v>0.1</v>
+        <v>0.108</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -1192,10 +1192,10 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0.099</v>
+        <v>0.105</v>
       </c>
       <c r="L6">
-        <v>0.099</v>
+        <v>0.105</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1236,10 +1236,10 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0.12</v>
+        <v>0.126</v>
       </c>
       <c r="L7">
-        <v>0.12</v>
+        <v>0.126</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1280,10 +1280,10 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0.028</v>
+        <v>0.03</v>
       </c>
       <c r="L8">
-        <v>0.028</v>
+        <v>0.03</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1324,10 +1324,10 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0.023</v>
+        <v>0.024</v>
       </c>
       <c r="L9">
-        <v>0.023</v>
+        <v>0.024</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1368,10 +1368,10 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0.028</v>
+        <v>0.029</v>
       </c>
       <c r="L10">
-        <v>0.028</v>
+        <v>0.029</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1502,10 +1502,10 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>11.904</v>
+        <v>11.864</v>
       </c>
       <c r="I2">
-        <v>0.031</v>
+        <v>0.034</v>
       </c>
       <c r="J2">
         <v>2.38</v>
@@ -1526,10 +1526,10 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.516</v>
+        <v>0.556</v>
       </c>
       <c r="Q2">
-        <v>0.031</v>
+        <v>0.034</v>
       </c>
       <c r="R2">
         <v>5.45</v>
@@ -1588,10 +1588,10 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>11.539</v>
+        <v>11.471</v>
       </c>
       <c r="I3">
-        <v>0.035</v>
+        <v>0.037</v>
       </c>
       <c r="J3">
         <v>2.38</v>
@@ -1612,10 +1612,10 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.881</v>
+        <v>0.948</v>
       </c>
       <c r="Q3">
-        <v>0.035</v>
+        <v>0.037</v>
       </c>
       <c r="R3">
         <v>5.45</v>
@@ -1674,10 +1674,10 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>11.358</v>
+        <v>11.277</v>
       </c>
       <c r="I4">
-        <v>0.043</v>
+        <v>0.044</v>
       </c>
       <c r="J4">
         <v>2.38</v>
@@ -1698,10 +1698,10 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>1.061</v>
+        <v>1.143</v>
       </c>
       <c r="Q4">
-        <v>0.043</v>
+        <v>0.044</v>
       </c>
       <c r="R4">
         <v>5.45</v>
@@ -1760,10 +1760,10 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>13.226</v>
+        <v>13.211</v>
       </c>
       <c r="I5">
-        <v>0.1</v>
+        <v>0.108</v>
       </c>
       <c r="J5">
         <v>2.39</v>
@@ -1784,10 +1784,10 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.203</v>
+        <v>0.219</v>
       </c>
       <c r="Q5">
-        <v>0.1</v>
+        <v>0.108</v>
       </c>
       <c r="R5">
         <v>5.4</v>
@@ -1846,10 +1846,10 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>12.873</v>
+        <v>12.828</v>
       </c>
       <c r="I6">
-        <v>0.099</v>
+        <v>0.105</v>
       </c>
       <c r="J6">
         <v>2.39</v>
@@ -1870,10 +1870,10 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.556</v>
+        <v>0.602</v>
       </c>
       <c r="Q6">
-        <v>0.099</v>
+        <v>0.105</v>
       </c>
       <c r="R6">
         <v>5.4</v>
@@ -1932,10 +1932,10 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>12.76</v>
+        <v>12.705</v>
       </c>
       <c r="I7">
-        <v>0.12</v>
+        <v>0.126</v>
       </c>
       <c r="J7">
         <v>2.39</v>
@@ -1956,10 +1956,10 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>0.67</v>
+        <v>0.725</v>
       </c>
       <c r="Q7">
-        <v>0.12</v>
+        <v>0.126</v>
       </c>
       <c r="R7">
         <v>5.4</v>
@@ -2018,10 +2018,10 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>7.866</v>
+        <v>7.82</v>
       </c>
       <c r="I8">
-        <v>0.028</v>
+        <v>0.03</v>
       </c>
       <c r="J8">
         <v>2.4</v>
@@ -2042,10 +2042,10 @@
         <v>0</v>
       </c>
       <c r="P8">
-        <v>0.603</v>
+        <v>0.649</v>
       </c>
       <c r="Q8">
-        <v>0.028</v>
+        <v>0.03</v>
       </c>
       <c r="R8">
         <v>6</v>
@@ -2104,10 +2104,10 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>7.495</v>
+        <v>7.417</v>
       </c>
       <c r="I9">
-        <v>0.023</v>
+        <v>0.024</v>
       </c>
       <c r="J9">
         <v>2.4</v>
@@ -2128,10 +2128,10 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>0.975</v>
+        <v>1.052</v>
       </c>
       <c r="Q9">
-        <v>0.023</v>
+        <v>0.024</v>
       </c>
       <c r="R9">
         <v>6</v>
@@ -2190,10 +2190,10 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>7.295</v>
+        <v>7.202</v>
       </c>
       <c r="I10">
-        <v>0.028</v>
+        <v>0.029</v>
       </c>
       <c r="J10">
         <v>2.4</v>
@@ -2214,10 +2214,10 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>1.174</v>
+        <v>1.267</v>
       </c>
       <c r="Q10">
-        <v>0.028</v>
+        <v>0.029</v>
       </c>
       <c r="R10">
         <v>6</v>

</xml_diff>